<commit_message>
Arreglo de modelo de Dominio
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/Clientes - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/Clientes - Muestreo Datos.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis ospina\OneDrive\Documentos\GitHub\DOO\SpaOnline\ModeloDominio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://grchia-my.sharepoint.com/personal/jhonatan_gomez_wiga_io/Documents/Escritorio/UCO/DOO/SpaOnline/ModeloDominio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B967F0-8C49-4A29-9527-9CC6D90121FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{19B967F0-8C49-4A29-9527-9CC6D90121FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8DC872E-98D9-43F3-B5F7-01114E9E8D0F}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
     <sheet name="Objetos de dominio" sheetId="2" r:id="rId2"/>
     <sheet name="Cliente" sheetId="5" r:id="rId3"/>
-    <sheet name="TipoIdentificacion" sheetId="6" r:id="rId4"/>
+    <sheet name="Genero" sheetId="7" r:id="rId4"/>
+    <sheet name="TipoIdentificacion" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -158,13 +159,25 @@
   </si>
   <si>
     <t>InformacionBase</t>
+  </si>
+  <si>
+    <t>Genero</t>
+  </si>
+  <si>
+    <t>Masculino</t>
+  </si>
+  <si>
+    <t>Femenino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objeto de dominio que contiene la informacion de genero del cliente </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,6 +197,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -260,6 +281,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -288,17 +311,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>448695</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>48110</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>39169</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>425</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A118857-CACD-4233-A2D8-4AFC78D8CFDB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82571E10-C5E0-DBA5-3A0B-91FA856DE467}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -315,7 +338,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7306695" cy="3477110"/>
+          <a:ext cx="7659169" cy="3048425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -660,17 +683,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA198BEE-AB41-4447-8B76-5672FB9C01F4}">
-  <dimension ref="A1"/>
+  <dimension ref="L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="11.42578125" style="7"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="13" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L13" s="12"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -678,10 +705,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D92343-C7F8-498A-9249-704487594109}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,17 +747,31 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
     </row>
@@ -742,21 +783,157 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G1" sqref="A1:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>+TipoIdentificacion!B7</f>
+        <v>CC</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>Genero!B3</f>
+        <v>Femenino</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1234567890</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3116987523</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="5" t="str">
+        <f>+B2&amp;"-"&amp;E2</f>
+        <v>Martina Corrales-1234567890</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>+TipoIdentificacion!B8</f>
+        <v>Pasaporte</v>
+      </c>
+      <c r="D3" s="1" t="str">
+        <f>Genero!B2</f>
+        <v>Masculino</v>
+      </c>
+      <c r="E3" s="1">
+        <v>987654321</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3639874520</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="5" t="str">
+        <f t="shared" ref="H3:H4" si="0">+B3&amp;"-"&amp;E3</f>
+        <v>Ramiro Ramirez-987654321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>+TipoIdentificacion!B9</f>
+        <v>TI</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f>Genero!B3</f>
+        <v>Femenino</v>
+      </c>
+      <c r="E4" s="1">
+        <v>39789321</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3793175677</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Lucrecia Gomez-39789321</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G4" r:id="rId1" xr:uid="{AA19E663-C136-4DC8-8636-967DE1057D4A}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{99325E93-3349-475B-9142-1A909A776246}"/>
+    <hyperlink ref="G2" r:id="rId3" xr:uid="{532774D5-0E4A-4D14-85D2-644383B16386}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C1D11C-26CD-40E3-B239-1679473BEA61}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -764,21 +941,9 @@
         <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -787,24 +952,11 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="1" t="str">
-        <f>+TipoIdentificacion!B7</f>
-        <v>CC</v>
-      </c>
-      <c r="D2" s="1">
-        <v>1234567890</v>
-      </c>
-      <c r="E2" s="1">
-        <v>3116987523</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="5" t="str">
-        <f>+B2&amp;"-"&amp;D2</f>
-        <v>Martina Corrales-1234567890</v>
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>B2</f>
+        <v>Masculino</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -812,67 +964,27 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="1" t="str">
-        <f>+TipoIdentificacion!B8</f>
-        <v>Pasaporte</v>
-      </c>
-      <c r="D3" s="1">
-        <v>987654321</v>
-      </c>
-      <c r="E3" s="1">
-        <v>3639874520</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="5" t="str">
-        <f t="shared" ref="G3:G4" si="0">+B3&amp;"-"&amp;D3</f>
-        <v>Ramiro Ramirez-987654321</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="1" t="str">
-        <f>+TipoIdentificacion!B9</f>
-        <v>TI</v>
-      </c>
-      <c r="D4" s="1">
-        <v>39789321</v>
-      </c>
-      <c r="E4" s="1">
-        <v>3793175677</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>Lucrecia Gomez-39789321</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f>B3</f>
+        <v>Femenino</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G8" s="13"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F4" r:id="rId1" xr:uid="{AA19E663-C136-4DC8-8636-967DE1057D4A}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{99325E93-3349-475B-9142-1A909A776246}"/>
-    <hyperlink ref="F2" r:id="rId3" xr:uid="{532774D5-0E4A-4D14-85D2-644383B16386}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD872A8-E9F6-4C5D-A950-6E293C692F23}">
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrección errores muestreo de datos
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/Clientes - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/Clientes - Muestreo Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\SpaOnline\ModeloDominio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0C9389-CD41-48CB-B50C-0114AD594E29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{988BC905-92EB-4B4D-819B-AA92F56D98AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="4" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
@@ -790,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,8 +988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAD872A8-E9F6-4C5D-A950-6E293C692F23}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>